<commit_message>
Frontend Form connected with backend.
Path Variable added
</commit_message>
<xml_diff>
--- a/ExcelFSTemplate.xlsx
+++ b/ExcelFSTemplate.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Python Projects\VTU-Marks-Extraction-\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VTU-Marks-Extraction-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96EF9243-30AF-4ACB-9592-81B48C079F74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CBF13FC-2B7C-4F4F-A77B-F8BCD82701AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -250,6 +250,12 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -274,12 +280,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -597,7 +597,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,42 +610,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="14"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="9"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="11"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="13" t="s">
+      <c r="A3" s="19"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="15"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="17"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="20"/>
+      <c r="A4" s="20"/>
+      <c r="B4" s="8"/>
       <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
@@ -677,7 +677,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,42 +690,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="14"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="9"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="11"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="13" t="s">
+      <c r="A3" s="19"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="15"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="17"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="20"/>
+      <c r="A4" s="20"/>
+      <c r="B4" s="8"/>
       <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
@@ -757,7 +757,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -770,42 +770,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="14"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="9"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="11"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="13" t="s">
+      <c r="A3" s="19"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="15"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="17"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="20"/>
+      <c r="A4" s="20"/>
+      <c r="B4" s="8"/>
       <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
@@ -837,7 +837,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -850,42 +850,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="14"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="9"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="11"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="13" t="s">
+      <c r="A3" s="19"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="15"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="17"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="20"/>
+      <c r="A4" s="20"/>
+      <c r="B4" s="8"/>
       <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
@@ -917,7 +917,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -930,42 +930,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="14"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="9"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="11"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="13" t="s">
+      <c r="A3" s="19"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="15"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="17"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="20"/>
+      <c r="A4" s="20"/>
+      <c r="B4" s="8"/>
       <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
@@ -997,7 +997,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1010,42 +1010,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="14"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="9"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="11"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="13" t="s">
+      <c r="A3" s="19"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="15"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="17"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="20"/>
+      <c r="A4" s="20"/>
+      <c r="B4" s="8"/>
       <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1077,7 +1077,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F1:F1048576"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1090,42 +1090,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="14"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="9"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="11"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="13" t="s">
+      <c r="A3" s="19"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="15"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="17"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="20"/>
+      <c r="A4" s="20"/>
+      <c r="B4" s="8"/>
       <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1157,7 +1157,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1170,42 +1170,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="14"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="9"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="11"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="13" t="s">
+      <c r="A3" s="19"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="15"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="17"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="20"/>
+      <c r="A4" s="20"/>
+      <c r="B4" s="8"/>
       <c r="C4" s="1" t="s">
         <v>2</v>
       </c>

</xml_diff>